<commit_message>
Incorporating final PMLS data of 2021-07-27, final check-over the week before publication
</commit_message>
<xml_diff>
--- a/data/dataPaper-I-in/arphified/Arthropoda.xlsx
+++ b/data/dataPaper-I-in/arphified/Arthropoda.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3250" uniqueCount="622">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3284" uniqueCount="624">
   <si>
     <t>Taxon_Local_ID</t>
   </si>
@@ -1027,6 +1027,12 @@
   </si>
   <si>
     <t>(Rathbun, 1902)</t>
+  </si>
+  <si>
+    <t>67627</t>
+  </si>
+  <si>
+    <t>(J.F. Brandt in von Middendorf, 1851)</t>
   </si>
   <si>
     <t>458674</t>
@@ -2255,7 +2261,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH86"/>
+  <dimension ref="A1:AH87"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.25">
@@ -9285,19 +9291,19 @@
         <v>36</v>
       </c>
       <c r="T68" t="s">
+        <v>203</v>
+      </c>
+      <c r="U68" t="s">
+        <v>36</v>
+      </c>
+      <c r="V68" t="s">
+        <v>36</v>
+      </c>
+      <c r="W68" t="s">
+        <v>36</v>
+      </c>
+      <c r="X68" t="s">
         <v>339</v>
-      </c>
-      <c r="U68" t="s">
-        <v>36</v>
-      </c>
-      <c r="V68" t="s">
-        <v>36</v>
-      </c>
-      <c r="W68" t="s">
-        <v>36</v>
-      </c>
-      <c r="X68" t="s">
-        <v>246</v>
       </c>
       <c r="Y68" t="s">
         <v>36</v>
@@ -9401,7 +9407,7 @@
         <v>36</v>
       </c>
       <c r="X69" t="s">
-        <v>337</v>
+        <v>246</v>
       </c>
       <c r="Y69" t="s">
         <v>36</v>
@@ -9487,14 +9493,14 @@
         <v>36</v>
       </c>
       <c r="R70" t="s">
+        <v>333</v>
+      </c>
+      <c r="S70" t="s">
+        <v>36</v>
+      </c>
+      <c r="T70" t="s">
         <v>343</v>
       </c>
-      <c r="S70" t="s">
-        <v>36</v>
-      </c>
-      <c r="T70" t="s">
-        <v>344</v>
-      </c>
       <c r="U70" t="s">
         <v>36</v>
       </c>
@@ -9505,7 +9511,7 @@
         <v>36</v>
       </c>
       <c r="X70" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
       <c r="Y70" t="s">
         <v>36</v>
@@ -9540,7 +9546,7 @@
     </row>
     <row r="71" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B71" t="s">
         <v>35</v>
@@ -9591,25 +9597,25 @@
         <v>36</v>
       </c>
       <c r="R71" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="S71" t="s">
         <v>36</v>
       </c>
       <c r="T71" t="s">
+        <v>346</v>
+      </c>
+      <c r="U71" t="s">
+        <v>36</v>
+      </c>
+      <c r="V71" t="s">
+        <v>36</v>
+      </c>
+      <c r="W71" t="s">
+        <v>36</v>
+      </c>
+      <c r="X71" t="s">
         <v>347</v>
-      </c>
-      <c r="U71" t="s">
-        <v>36</v>
-      </c>
-      <c r="V71" t="s">
-        <v>36</v>
-      </c>
-      <c r="W71" t="s">
-        <v>36</v>
-      </c>
-      <c r="X71" t="s">
-        <v>348</v>
       </c>
       <c r="Y71" t="s">
         <v>36</v>
@@ -9644,7 +9650,7 @@
     </row>
     <row r="72" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B72" t="s">
         <v>35</v>
@@ -9695,25 +9701,25 @@
         <v>36</v>
       </c>
       <c r="R72" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="S72" t="s">
         <v>36</v>
       </c>
       <c r="T72" t="s">
+        <v>349</v>
+      </c>
+      <c r="U72" t="s">
+        <v>36</v>
+      </c>
+      <c r="V72" t="s">
+        <v>36</v>
+      </c>
+      <c r="W72" t="s">
+        <v>36</v>
+      </c>
+      <c r="X72" t="s">
         <v>350</v>
-      </c>
-      <c r="U72" t="s">
-        <v>36</v>
-      </c>
-      <c r="V72" t="s">
-        <v>36</v>
-      </c>
-      <c r="W72" t="s">
-        <v>36</v>
-      </c>
-      <c r="X72" t="s">
-        <v>345</v>
       </c>
       <c r="Y72" t="s">
         <v>36</v>
@@ -9799,14 +9805,14 @@
         <v>36</v>
       </c>
       <c r="R73" t="s">
+        <v>345</v>
+      </c>
+      <c r="S73" t="s">
+        <v>36</v>
+      </c>
+      <c r="T73" t="s">
         <v>352</v>
       </c>
-      <c r="S73" t="s">
-        <v>36</v>
-      </c>
-      <c r="T73" t="s">
-        <v>353</v>
-      </c>
       <c r="U73" t="s">
         <v>36</v>
       </c>
@@ -9817,7 +9823,7 @@
         <v>36</v>
       </c>
       <c r="X73" t="s">
-        <v>246</v>
+        <v>347</v>
       </c>
       <c r="Y73" t="s">
         <v>36</v>
@@ -9852,7 +9858,7 @@
     </row>
     <row r="74" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B74" t="s">
         <v>35</v>
@@ -9888,29 +9894,29 @@
         <v>326</v>
       </c>
       <c r="M74" t="s">
+        <v>327</v>
+      </c>
+      <c r="N74" t="s">
+        <v>328</v>
+      </c>
+      <c r="O74" t="s">
+        <v>36</v>
+      </c>
+      <c r="P74" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q74" t="s">
+        <v>36</v>
+      </c>
+      <c r="R74" t="s">
+        <v>354</v>
+      </c>
+      <c r="S74" t="s">
+        <v>36</v>
+      </c>
+      <c r="T74" t="s">
         <v>355</v>
       </c>
-      <c r="N74" t="s">
-        <v>356</v>
-      </c>
-      <c r="O74" t="s">
-        <v>36</v>
-      </c>
-      <c r="P74" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q74" t="s">
-        <v>36</v>
-      </c>
-      <c r="R74" t="s">
-        <v>357</v>
-      </c>
-      <c r="S74" t="s">
-        <v>36</v>
-      </c>
-      <c r="T74" t="s">
-        <v>358</v>
-      </c>
       <c r="U74" t="s">
         <v>36</v>
       </c>
@@ -9921,7 +9927,7 @@
         <v>36</v>
       </c>
       <c r="X74" t="s">
-        <v>359</v>
+        <v>246</v>
       </c>
       <c r="Y74" t="s">
         <v>36</v>
@@ -9956,7 +9962,7 @@
     </row>
     <row r="75" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="B75" t="s">
         <v>35</v>
@@ -9992,10 +9998,10 @@
         <v>326</v>
       </c>
       <c r="M75" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="N75" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="O75" t="s">
         <v>36</v>
@@ -10007,25 +10013,25 @@
         <v>36</v>
       </c>
       <c r="R75" t="s">
+        <v>359</v>
+      </c>
+      <c r="S75" t="s">
+        <v>36</v>
+      </c>
+      <c r="T75" t="s">
+        <v>360</v>
+      </c>
+      <c r="U75" t="s">
+        <v>36</v>
+      </c>
+      <c r="V75" t="s">
+        <v>36</v>
+      </c>
+      <c r="W75" t="s">
+        <v>36</v>
+      </c>
+      <c r="X75" t="s">
         <v>361</v>
-      </c>
-      <c r="S75" t="s">
-        <v>36</v>
-      </c>
-      <c r="T75" t="s">
-        <v>362</v>
-      </c>
-      <c r="U75" t="s">
-        <v>36</v>
-      </c>
-      <c r="V75" t="s">
-        <v>36</v>
-      </c>
-      <c r="W75" t="s">
-        <v>36</v>
-      </c>
-      <c r="X75" t="s">
-        <v>272</v>
       </c>
       <c r="Y75" t="s">
         <v>36</v>
@@ -10060,7 +10066,7 @@
     </row>
     <row r="76" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B76" t="s">
         <v>35</v>
@@ -10096,29 +10102,29 @@
         <v>326</v>
       </c>
       <c r="M76" t="s">
+        <v>357</v>
+      </c>
+      <c r="N76" t="s">
+        <v>358</v>
+      </c>
+      <c r="O76" t="s">
+        <v>36</v>
+      </c>
+      <c r="P76" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q76" t="s">
+        <v>36</v>
+      </c>
+      <c r="R76" t="s">
+        <v>363</v>
+      </c>
+      <c r="S76" t="s">
+        <v>36</v>
+      </c>
+      <c r="T76" t="s">
         <v>364</v>
       </c>
-      <c r="N76" t="s">
-        <v>365</v>
-      </c>
-      <c r="O76" t="s">
-        <v>36</v>
-      </c>
-      <c r="P76" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q76" t="s">
-        <v>36</v>
-      </c>
-      <c r="R76" t="s">
-        <v>366</v>
-      </c>
-      <c r="S76" t="s">
-        <v>36</v>
-      </c>
-      <c r="T76" t="s">
-        <v>367</v>
-      </c>
       <c r="U76" t="s">
         <v>36</v>
       </c>
@@ -10129,7 +10135,7 @@
         <v>36</v>
       </c>
       <c r="X76" t="s">
-        <v>368</v>
+        <v>272</v>
       </c>
       <c r="Y76" t="s">
         <v>36</v>
@@ -10164,7 +10170,7 @@
     </row>
     <row r="77" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="B77" t="s">
         <v>35</v>
@@ -10200,10 +10206,10 @@
         <v>326</v>
       </c>
       <c r="M77" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="N77" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="O77" t="s">
         <v>36</v>
@@ -10215,25 +10221,25 @@
         <v>36</v>
       </c>
       <c r="R77" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="S77" t="s">
         <v>36</v>
       </c>
       <c r="T77" t="s">
+        <v>369</v>
+      </c>
+      <c r="U77" t="s">
+        <v>36</v>
+      </c>
+      <c r="V77" t="s">
+        <v>36</v>
+      </c>
+      <c r="W77" t="s">
+        <v>36</v>
+      </c>
+      <c r="X77" t="s">
         <v>370</v>
-      </c>
-      <c r="U77" t="s">
-        <v>36</v>
-      </c>
-      <c r="V77" t="s">
-        <v>36</v>
-      </c>
-      <c r="W77" t="s">
-        <v>36</v>
-      </c>
-      <c r="X77" t="s">
-        <v>371</v>
       </c>
       <c r="Y77" t="s">
         <v>36</v>
@@ -10268,7 +10274,7 @@
     </row>
     <row r="78" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B78" t="s">
         <v>35</v>
@@ -10304,10 +10310,10 @@
         <v>326</v>
       </c>
       <c r="M78" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="N78" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="O78" t="s">
         <v>36</v>
@@ -10319,25 +10325,25 @@
         <v>36</v>
       </c>
       <c r="R78" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="S78" t="s">
         <v>36</v>
       </c>
       <c r="T78" t="s">
+        <v>372</v>
+      </c>
+      <c r="U78" t="s">
+        <v>36</v>
+      </c>
+      <c r="V78" t="s">
+        <v>36</v>
+      </c>
+      <c r="W78" t="s">
+        <v>36</v>
+      </c>
+      <c r="X78" t="s">
         <v>373</v>
-      </c>
-      <c r="U78" t="s">
-        <v>36</v>
-      </c>
-      <c r="V78" t="s">
-        <v>36</v>
-      </c>
-      <c r="W78" t="s">
-        <v>36</v>
-      </c>
-      <c r="X78" t="s">
-        <v>374</v>
       </c>
       <c r="Y78" t="s">
         <v>36</v>
@@ -10372,7 +10378,7 @@
     </row>
     <row r="79" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B79" t="s">
         <v>35</v>
@@ -10408,10 +10414,10 @@
         <v>326</v>
       </c>
       <c r="M79" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="N79" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="O79" t="s">
         <v>36</v>
@@ -10423,26 +10429,26 @@
         <v>36</v>
       </c>
       <c r="R79" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="S79" t="s">
         <v>36</v>
       </c>
       <c r="T79" t="s">
+        <v>375</v>
+      </c>
+      <c r="U79" t="s">
+        <v>36</v>
+      </c>
+      <c r="V79" t="s">
+        <v>36</v>
+      </c>
+      <c r="W79" t="s">
+        <v>36</v>
+      </c>
+      <c r="X79" t="s">
         <v>376</v>
       </c>
-      <c r="U79" t="s">
-        <v>36</v>
-      </c>
-      <c r="V79" t="s">
-        <v>36</v>
-      </c>
-      <c r="W79" t="s">
-        <v>36</v>
-      </c>
-      <c r="X79" t="s">
-        <v>377</v>
-      </c>
       <c r="Y79" t="s">
         <v>36</v>
       </c>
@@ -10471,12 +10477,12 @@
         <v>36</v>
       </c>
       <c r="AH79" t="s">
-        <v>378</v>
+        <v>36</v>
       </c>
     </row>
     <row r="80" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B80" t="s">
         <v>35</v>
@@ -10512,10 +10518,10 @@
         <v>326</v>
       </c>
       <c r="M80" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="N80" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="O80" t="s">
         <v>36</v>
@@ -10527,60 +10533,60 @@
         <v>36</v>
       </c>
       <c r="R80" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="S80" t="s">
         <v>36</v>
       </c>
       <c r="T80" t="s">
+        <v>378</v>
+      </c>
+      <c r="U80" t="s">
+        <v>36</v>
+      </c>
+      <c r="V80" t="s">
+        <v>36</v>
+      </c>
+      <c r="W80" t="s">
+        <v>36</v>
+      </c>
+      <c r="X80" t="s">
+        <v>379</v>
+      </c>
+      <c r="Y80" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z80" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA80" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB80" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC80" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD80" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE80" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF80" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG80" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH80" t="s">
         <v>380</v>
-      </c>
-      <c r="U80" t="s">
-        <v>36</v>
-      </c>
-      <c r="V80" t="s">
-        <v>36</v>
-      </c>
-      <c r="W80" t="s">
-        <v>36</v>
-      </c>
-      <c r="X80" t="s">
-        <v>381</v>
-      </c>
-      <c r="Y80" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z80" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA80" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB80" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC80" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD80" t="s">
-        <v>36</v>
-      </c>
-      <c r="AE80" t="s">
-        <v>36</v>
-      </c>
-      <c r="AF80" t="s">
-        <v>36</v>
-      </c>
-      <c r="AG80" t="s">
-        <v>36</v>
-      </c>
-      <c r="AH80" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="81" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B81" t="s">
         <v>35</v>
@@ -10616,10 +10622,10 @@
         <v>326</v>
       </c>
       <c r="M81" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="N81" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="O81" t="s">
         <v>36</v>
@@ -10631,25 +10637,25 @@
         <v>36</v>
       </c>
       <c r="R81" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="S81" t="s">
         <v>36</v>
       </c>
       <c r="T81" t="s">
+        <v>382</v>
+      </c>
+      <c r="U81" t="s">
+        <v>36</v>
+      </c>
+      <c r="V81" t="s">
+        <v>36</v>
+      </c>
+      <c r="W81" t="s">
+        <v>36</v>
+      </c>
+      <c r="X81" t="s">
         <v>383</v>
-      </c>
-      <c r="U81" t="s">
-        <v>36</v>
-      </c>
-      <c r="V81" t="s">
-        <v>36</v>
-      </c>
-      <c r="W81" t="s">
-        <v>36</v>
-      </c>
-      <c r="X81" t="s">
-        <v>384</v>
       </c>
       <c r="Y81" t="s">
         <v>36</v>
@@ -10684,7 +10690,7 @@
     </row>
     <row r="82" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B82" t="s">
         <v>35</v>
@@ -10711,50 +10717,50 @@
         <v>161</v>
       </c>
       <c r="J82" t="s">
+        <v>162</v>
+      </c>
+      <c r="K82" t="s">
+        <v>171</v>
+      </c>
+      <c r="L82" t="s">
+        <v>326</v>
+      </c>
+      <c r="M82" t="s">
+        <v>366</v>
+      </c>
+      <c r="N82" t="s">
+        <v>367</v>
+      </c>
+      <c r="O82" t="s">
+        <v>36</v>
+      </c>
+      <c r="P82" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q82" t="s">
+        <v>36</v>
+      </c>
+      <c r="R82" t="s">
+        <v>368</v>
+      </c>
+      <c r="S82" t="s">
+        <v>36</v>
+      </c>
+      <c r="T82" t="s">
+        <v>385</v>
+      </c>
+      <c r="U82" t="s">
+        <v>36</v>
+      </c>
+      <c r="V82" t="s">
+        <v>36</v>
+      </c>
+      <c r="W82" t="s">
+        <v>36</v>
+      </c>
+      <c r="X82" t="s">
         <v>386</v>
       </c>
-      <c r="K82" t="s">
-        <v>36</v>
-      </c>
-      <c r="L82" t="s">
-        <v>36</v>
-      </c>
-      <c r="M82" t="s">
-        <v>36</v>
-      </c>
-      <c r="N82" t="s">
-        <v>387</v>
-      </c>
-      <c r="O82" t="s">
-        <v>36</v>
-      </c>
-      <c r="P82" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q82" t="s">
-        <v>36</v>
-      </c>
-      <c r="R82" t="s">
-        <v>388</v>
-      </c>
-      <c r="S82" t="s">
-        <v>36</v>
-      </c>
-      <c r="T82" t="s">
-        <v>389</v>
-      </c>
-      <c r="U82" t="s">
-        <v>36</v>
-      </c>
-      <c r="V82" t="s">
-        <v>36</v>
-      </c>
-      <c r="W82" t="s">
-        <v>36</v>
-      </c>
-      <c r="X82" t="s">
-        <v>36</v>
-      </c>
       <c r="Y82" t="s">
         <v>36</v>
       </c>
@@ -10783,12 +10789,12 @@
         <v>36</v>
       </c>
       <c r="AH82" t="s">
-        <v>390</v>
+        <v>36</v>
       </c>
     </row>
     <row r="83" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="B83" t="s">
         <v>35</v>
@@ -10812,87 +10818,87 @@
         <v>87</v>
       </c>
       <c r="I83" t="s">
-        <v>88</v>
+        <v>161</v>
       </c>
       <c r="J83" t="s">
+        <v>388</v>
+      </c>
+      <c r="K83" t="s">
+        <v>36</v>
+      </c>
+      <c r="L83" t="s">
+        <v>36</v>
+      </c>
+      <c r="M83" t="s">
+        <v>36</v>
+      </c>
+      <c r="N83" t="s">
+        <v>389</v>
+      </c>
+      <c r="O83" t="s">
+        <v>36</v>
+      </c>
+      <c r="P83" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q83" t="s">
+        <v>36</v>
+      </c>
+      <c r="R83" t="s">
+        <v>390</v>
+      </c>
+      <c r="S83" t="s">
+        <v>36</v>
+      </c>
+      <c r="T83" t="s">
+        <v>391</v>
+      </c>
+      <c r="U83" t="s">
+        <v>36</v>
+      </c>
+      <c r="V83" t="s">
+        <v>36</v>
+      </c>
+      <c r="W83" t="s">
+        <v>36</v>
+      </c>
+      <c r="X83" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y83" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z83" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA83" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB83" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC83" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD83" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE83" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF83" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG83" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH83" t="s">
         <v>392</v>
-      </c>
-      <c r="K83" t="s">
-        <v>393</v>
-      </c>
-      <c r="L83" t="s">
-        <v>394</v>
-      </c>
-      <c r="M83" t="s">
-        <v>395</v>
-      </c>
-      <c r="N83" t="s">
-        <v>396</v>
-      </c>
-      <c r="O83" t="s">
-        <v>397</v>
-      </c>
-      <c r="P83" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q83" t="s">
-        <v>36</v>
-      </c>
-      <c r="R83" t="s">
-        <v>398</v>
-      </c>
-      <c r="S83" t="s">
-        <v>36</v>
-      </c>
-      <c r="T83" t="s">
-        <v>399</v>
-      </c>
-      <c r="U83" t="s">
-        <v>36</v>
-      </c>
-      <c r="V83" t="s">
-        <v>36</v>
-      </c>
-      <c r="W83" t="s">
-        <v>36</v>
-      </c>
-      <c r="X83" t="s">
-        <v>400</v>
-      </c>
-      <c r="Y83" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z83" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA83" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB83" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC83" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD83" t="s">
-        <v>36</v>
-      </c>
-      <c r="AE83" t="s">
-        <v>36</v>
-      </c>
-      <c r="AF83" t="s">
-        <v>36</v>
-      </c>
-      <c r="AG83" t="s">
-        <v>36</v>
-      </c>
-      <c r="AH83" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="84" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
       <c r="B84" t="s">
         <v>35</v>
@@ -10919,49 +10925,49 @@
         <v>88</v>
       </c>
       <c r="J84" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="K84" t="s">
+        <v>395</v>
+      </c>
+      <c r="L84" t="s">
+        <v>396</v>
+      </c>
+      <c r="M84" t="s">
+        <v>397</v>
+      </c>
+      <c r="N84" t="s">
+        <v>398</v>
+      </c>
+      <c r="O84" t="s">
+        <v>399</v>
+      </c>
+      <c r="P84" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q84" t="s">
+        <v>36</v>
+      </c>
+      <c r="R84" t="s">
+        <v>400</v>
+      </c>
+      <c r="S84" t="s">
+        <v>36</v>
+      </c>
+      <c r="T84" t="s">
+        <v>401</v>
+      </c>
+      <c r="U84" t="s">
+        <v>36</v>
+      </c>
+      <c r="V84" t="s">
+        <v>36</v>
+      </c>
+      <c r="W84" t="s">
+        <v>36</v>
+      </c>
+      <c r="X84" t="s">
         <v>402</v>
-      </c>
-      <c r="L84" t="s">
-        <v>36</v>
-      </c>
-      <c r="M84" t="s">
-        <v>403</v>
-      </c>
-      <c r="N84" t="s">
-        <v>404</v>
-      </c>
-      <c r="O84" t="s">
-        <v>36</v>
-      </c>
-      <c r="P84" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q84" t="s">
-        <v>36</v>
-      </c>
-      <c r="R84" t="s">
-        <v>405</v>
-      </c>
-      <c r="S84" t="s">
-        <v>36</v>
-      </c>
-      <c r="T84" t="s">
-        <v>406</v>
-      </c>
-      <c r="U84" t="s">
-        <v>36</v>
-      </c>
-      <c r="V84" t="s">
-        <v>36</v>
-      </c>
-      <c r="W84" t="s">
-        <v>36</v>
-      </c>
-      <c r="X84" t="s">
-        <v>407</v>
       </c>
       <c r="Y84" t="s">
         <v>36</v>
@@ -10996,7 +11002,7 @@
     </row>
     <row r="85" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="B85" t="s">
         <v>35</v>
@@ -11023,49 +11029,49 @@
         <v>88</v>
       </c>
       <c r="J85" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="K85" t="s">
+        <v>404</v>
+      </c>
+      <c r="L85" t="s">
+        <v>36</v>
+      </c>
+      <c r="M85" t="s">
+        <v>405</v>
+      </c>
+      <c r="N85" t="s">
+        <v>406</v>
+      </c>
+      <c r="O85" t="s">
+        <v>36</v>
+      </c>
+      <c r="P85" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q85" t="s">
+        <v>36</v>
+      </c>
+      <c r="R85" t="s">
+        <v>407</v>
+      </c>
+      <c r="S85" t="s">
+        <v>36</v>
+      </c>
+      <c r="T85" t="s">
+        <v>408</v>
+      </c>
+      <c r="U85" t="s">
+        <v>36</v>
+      </c>
+      <c r="V85" t="s">
+        <v>36</v>
+      </c>
+      <c r="W85" t="s">
+        <v>36</v>
+      </c>
+      <c r="X85" t="s">
         <v>409</v>
-      </c>
-      <c r="L85" t="s">
-        <v>36</v>
-      </c>
-      <c r="M85" t="s">
-        <v>36</v>
-      </c>
-      <c r="N85" t="s">
-        <v>410</v>
-      </c>
-      <c r="O85" t="s">
-        <v>36</v>
-      </c>
-      <c r="P85" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q85" t="s">
-        <v>36</v>
-      </c>
-      <c r="R85" t="s">
-        <v>411</v>
-      </c>
-      <c r="S85" t="s">
-        <v>36</v>
-      </c>
-      <c r="T85" t="s">
-        <v>412</v>
-      </c>
-      <c r="U85" t="s">
-        <v>36</v>
-      </c>
-      <c r="V85" t="s">
-        <v>36</v>
-      </c>
-      <c r="W85" t="s">
-        <v>36</v>
-      </c>
-      <c r="X85" t="s">
-        <v>159</v>
       </c>
       <c r="Y85" t="s">
         <v>36</v>
@@ -11100,7 +11106,7 @@
     </row>
     <row r="86" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="B86" t="s">
         <v>35</v>
@@ -11127,10 +11133,10 @@
         <v>88</v>
       </c>
       <c r="J86" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="K86" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="L86" t="s">
         <v>36</v>
@@ -11139,7 +11145,7 @@
         <v>36</v>
       </c>
       <c r="N86" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="O86" t="s">
         <v>36</v>
@@ -11151,7 +11157,7 @@
         <v>36</v>
       </c>
       <c r="R86" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="S86" t="s">
         <v>36</v>
@@ -11169,36 +11175,140 @@
         <v>36</v>
       </c>
       <c r="X86" t="s">
+        <v>159</v>
+      </c>
+      <c r="Y86" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z86" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA86" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB86" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC86" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD86" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE86" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF86" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG86" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH86" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="87" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
         <v>415</v>
       </c>
-      <c r="Y86" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z86" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA86" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB86" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC86" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD86" t="s">
-        <v>36</v>
-      </c>
-      <c r="AE86" t="s">
-        <v>36</v>
-      </c>
-      <c r="AF86" t="s">
-        <v>36</v>
-      </c>
-      <c r="AG86" t="s">
-        <v>36</v>
-      </c>
-      <c r="AH86" t="s">
+      <c r="B87" t="s">
+        <v>35</v>
+      </c>
+      <c r="C87" t="s">
+        <v>36</v>
+      </c>
+      <c r="D87" t="s">
+        <v>37</v>
+      </c>
+      <c r="E87" t="s">
+        <v>38</v>
+      </c>
+      <c r="F87" t="s">
+        <v>39</v>
+      </c>
+      <c r="G87" t="s">
+        <v>86</v>
+      </c>
+      <c r="H87" t="s">
+        <v>87</v>
+      </c>
+      <c r="I87" t="s">
+        <v>88</v>
+      </c>
+      <c r="J87" t="s">
+        <v>394</v>
+      </c>
+      <c r="K87" t="s">
+        <v>411</v>
+      </c>
+      <c r="L87" t="s">
+        <v>36</v>
+      </c>
+      <c r="M87" t="s">
+        <v>36</v>
+      </c>
+      <c r="N87" t="s">
+        <v>412</v>
+      </c>
+      <c r="O87" t="s">
+        <v>36</v>
+      </c>
+      <c r="P87" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q87" t="s">
+        <v>36</v>
+      </c>
+      <c r="R87" t="s">
+        <v>413</v>
+      </c>
+      <c r="S87" t="s">
+        <v>36</v>
+      </c>
+      <c r="T87" t="s">
+        <v>416</v>
+      </c>
+      <c r="U87" t="s">
+        <v>36</v>
+      </c>
+      <c r="V87" t="s">
+        <v>36</v>
+      </c>
+      <c r="W87" t="s">
+        <v>36</v>
+      </c>
+      <c r="X87" t="s">
+        <v>417</v>
+      </c>
+      <c r="Y87" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z87" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA87" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB87" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC87" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD87" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE87" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF87" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG87" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH87" t="s">
         <v>36</v>
       </c>
     </row>
@@ -11218,495 +11328,495 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="C1" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="D1" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="E1" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="F1" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="G1" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="H1" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="I1" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="J1" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="K1" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="L1" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="M1" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="N1" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="O1" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="P1" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="Q1" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="R1" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="S1" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="T1" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="U1" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="V1" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="W1" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="X1" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="Y1" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="Z1" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="AA1" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="AB1" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="AC1" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="AD1" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="AE1" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="AF1" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="AG1" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="AH1" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="AI1" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="AJ1" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="AK1" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="AL1" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="AM1" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="AN1" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="AO1" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="AP1" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="AQ1" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="AR1" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="AS1" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="AT1" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="AU1" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="AV1" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="AW1" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="AX1" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="AY1" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="AZ1" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="BA1" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="BB1" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="BC1" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="BD1" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="BE1" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="BF1" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="BG1" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="BH1" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="BI1" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="BJ1" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="BK1" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="BL1" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="BM1" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="BN1" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="BO1" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="BP1" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="BQ1" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="BR1" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="BS1" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="BT1" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="BU1" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="BV1" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="BW1" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="BX1" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="BY1" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="BZ1" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="CA1" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="CB1" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c r="CC1" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="CD1" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="CE1" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="CF1" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="CG1" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="CH1" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="CI1" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c r="CJ1" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="CK1" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c r="CL1" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="CM1" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="CN1" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="CO1" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="CP1" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="CQ1" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="CR1" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="CS1" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c r="CT1" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
       <c r="CU1" t="s">
-        <v>513</v>
+        <v>515</v>
       </c>
       <c r="CV1" t="s">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="CW1" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="CX1" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="CY1" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="CZ1" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
       <c r="DA1" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c r="DB1" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="DC1" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="DD1" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="DE1" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="DF1" t="s">
-        <v>524</v>
+        <v>526</v>
       </c>
       <c r="DG1" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="DH1" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="DI1" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
       <c r="DJ1" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="DK1" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="DL1" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="DM1" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="DN1" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="DO1" t="s">
-        <v>533</v>
+        <v>535</v>
       </c>
       <c r="DP1" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
       <c r="DQ1" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="DR1" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="DS1" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c r="DT1" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="DU1" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="DV1" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="DW1" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="DX1" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="DY1" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
       <c r="DZ1" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="EA1" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
       <c r="EB1" t="s">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c r="EC1" t="s">
-        <v>547</v>
+        <v>549</v>
       </c>
       <c r="ED1" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="EE1" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="EF1" t="s">
-        <v>550</v>
+        <v>552</v>
       </c>
       <c r="EG1" t="s">
-        <v>551</v>
+        <v>553</v>
       </c>
       <c r="EH1" t="s">
-        <v>552</v>
+        <v>554</v>
       </c>
       <c r="EI1" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
       <c r="EJ1" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
       <c r="EK1" t="s">
-        <v>555</v>
+        <v>557</v>
       </c>
       <c r="EL1" t="s">
-        <v>556</v>
+        <v>558</v>
       </c>
       <c r="EM1" t="s">
-        <v>557</v>
+        <v>559</v>
       </c>
       <c r="EN1" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="EO1" t="s">
-        <v>559</v>
+        <v>561</v>
       </c>
       <c r="EP1" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="EQ1" t="s">
-        <v>561</v>
+        <v>563</v>
       </c>
       <c r="ER1" t="s">
-        <v>562</v>
+        <v>564</v>
       </c>
       <c r="ES1" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
       <c r="ET1" t="s">
-        <v>564</v>
+        <v>566</v>
       </c>
       <c r="EU1" t="s">
-        <v>565</v>
+        <v>567</v>
       </c>
       <c r="EV1" t="s">
-        <v>566</v>
+        <v>568</v>
       </c>
       <c r="EW1" t="s">
-        <v>567</v>
+        <v>569</v>
       </c>
       <c r="EX1" t="s">
-        <v>568</v>
+        <v>570</v>
       </c>
       <c r="EY1" t="s">
-        <v>569</v>
+        <v>571</v>
       </c>
       <c r="EZ1" t="s">
-        <v>570</v>
+        <v>572</v>
       </c>
       <c r="FA1" t="s">
-        <v>571</v>
+        <v>573</v>
       </c>
       <c r="FB1" t="s">
-        <v>572</v>
+        <v>574</v>
       </c>
       <c r="FC1" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="FD1" t="s">
-        <v>574</v>
+        <v>576</v>
       </c>
     </row>
     <row r="2" spans="1:160" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>575</v>
+        <v>577</v>
       </c>
       <c r="B2" t="s">
         <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>576</v>
+        <v>578</v>
       </c>
       <c r="D2" t="s">
-        <v>577</v>
+        <v>579</v>
       </c>
       <c r="E2" t="s">
         <v>36</v>
@@ -11718,428 +11828,428 @@
         <v>36</v>
       </c>
       <c r="H2" t="s">
-        <v>578</v>
+        <v>580</v>
       </c>
       <c r="I2" t="s">
         <v>36</v>
       </c>
       <c r="J2" t="s">
-        <v>579</v>
+        <v>581</v>
       </c>
       <c r="K2" t="s">
+        <v>582</v>
+      </c>
+      <c r="L2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M2" t="s">
+        <v>36</v>
+      </c>
+      <c r="N2" t="s">
+        <v>36</v>
+      </c>
+      <c r="O2" t="s">
+        <v>36</v>
+      </c>
+      <c r="P2" t="s">
+        <v>583</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>36</v>
+      </c>
+      <c r="R2" t="s">
+        <v>36</v>
+      </c>
+      <c r="S2" t="s">
+        <v>36</v>
+      </c>
+      <c r="T2" t="s">
+        <v>584</v>
+      </c>
+      <c r="U2" t="s">
+        <v>36</v>
+      </c>
+      <c r="V2" t="s">
+        <v>585</v>
+      </c>
+      <c r="W2" t="s">
+        <v>36</v>
+      </c>
+      <c r="X2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>586</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>587</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>588</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>589</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>590</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>591</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>592</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>593</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>594</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>595</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>596</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>597</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>598</v>
+      </c>
+      <c r="BC2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BE2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BF2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BG2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BH2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BI2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BJ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BK2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BL2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BM2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BN2" t="s">
+        <v>599</v>
+      </c>
+      <c r="BO2" t="s">
+        <v>600</v>
+      </c>
+      <c r="BP2" t="s">
+        <v>601</v>
+      </c>
+      <c r="BQ2" t="s">
+        <v>602</v>
+      </c>
+      <c r="BR2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BS2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BT2" t="s">
+        <v>603</v>
+      </c>
+      <c r="BU2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BV2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BW2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BX2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BY2" t="s">
+        <v>604</v>
+      </c>
+      <c r="BZ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CA2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CB2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CC2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CD2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CE2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CF2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CG2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CH2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CI2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CJ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CK2" t="s">
+        <v>605</v>
+      </c>
+      <c r="CL2" t="s">
+        <v>606</v>
+      </c>
+      <c r="CM2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CN2" t="s">
+        <v>607</v>
+      </c>
+      <c r="CO2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CP2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CQ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CR2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CS2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CT2" t="s">
         <v>580</v>
       </c>
-      <c r="L2" t="s">
-        <v>36</v>
-      </c>
-      <c r="M2" t="s">
-        <v>36</v>
-      </c>
-      <c r="N2" t="s">
-        <v>36</v>
-      </c>
-      <c r="O2" t="s">
-        <v>36</v>
-      </c>
-      <c r="P2" t="s">
-        <v>581</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>36</v>
-      </c>
-      <c r="R2" t="s">
-        <v>36</v>
-      </c>
-      <c r="S2" t="s">
-        <v>36</v>
-      </c>
-      <c r="T2" t="s">
-        <v>582</v>
-      </c>
-      <c r="U2" t="s">
-        <v>36</v>
-      </c>
-      <c r="V2" t="s">
-        <v>583</v>
-      </c>
-      <c r="W2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>584</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AG2" t="s">
+      <c r="CU2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CV2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CW2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CX2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CY2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CZ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DA2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DB2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DC2" t="s">
+        <v>608</v>
+      </c>
+      <c r="DD2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DE2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DF2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DG2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DH2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DI2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DJ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DK2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DL2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DM2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DN2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DO2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DP2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DQ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DR2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DS2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DT2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DU2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DV2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DW2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DX2" t="s">
+        <v>609</v>
+      </c>
+      <c r="DY2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DZ2" t="s">
+        <v>610</v>
+      </c>
+      <c r="EA2" t="s">
+        <v>611</v>
+      </c>
+      <c r="EB2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EC2" t="s">
+        <v>36</v>
+      </c>
+      <c r="ED2" t="s">
+        <v>612</v>
+      </c>
+      <c r="EE2" t="s">
+        <v>613</v>
+      </c>
+      <c r="EF2" t="s">
+        <v>614</v>
+      </c>
+      <c r="EG2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EH2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EI2" t="s">
+        <v>615</v>
+      </c>
+      <c r="EJ2" t="s">
+        <v>616</v>
+      </c>
+      <c r="EK2" t="s">
+        <v>617</v>
+      </c>
+      <c r="EL2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EM2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EN2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EO2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EP2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EQ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="ER2" t="s">
         <v>585</v>
       </c>
-      <c r="AH2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>586</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>587</v>
-      </c>
-      <c r="AP2" t="s">
-        <v>588</v>
-      </c>
-      <c r="AQ2" t="s">
-        <v>589</v>
-      </c>
-      <c r="AR2" t="s">
-        <v>590</v>
-      </c>
-      <c r="AS2" t="s">
-        <v>591</v>
-      </c>
-      <c r="AT2" t="s">
-        <v>592</v>
-      </c>
-      <c r="AU2" t="s">
-        <v>593</v>
-      </c>
-      <c r="AV2" t="s">
-        <v>594</v>
-      </c>
-      <c r="AW2" t="s">
-        <v>595</v>
-      </c>
-      <c r="AX2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AY2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AZ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BA2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BB2" t="s">
-        <v>596</v>
-      </c>
-      <c r="BC2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BD2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BE2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BF2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BG2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BH2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BI2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BJ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BK2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BL2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BM2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BN2" t="s">
-        <v>597</v>
-      </c>
-      <c r="BO2" t="s">
-        <v>598</v>
-      </c>
-      <c r="BP2" t="s">
-        <v>599</v>
-      </c>
-      <c r="BQ2" t="s">
-        <v>600</v>
-      </c>
-      <c r="BR2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BS2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BT2" t="s">
-        <v>601</v>
-      </c>
-      <c r="BU2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BV2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BW2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BX2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BY2" t="s">
-        <v>602</v>
-      </c>
-      <c r="BZ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CA2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CB2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CC2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CD2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CE2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CF2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CG2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CH2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CI2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CJ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CK2" t="s">
-        <v>603</v>
-      </c>
-      <c r="CL2" t="s">
-        <v>604</v>
-      </c>
-      <c r="CM2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CN2" t="s">
-        <v>605</v>
-      </c>
-      <c r="CO2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CP2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CQ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CR2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CS2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CT2" t="s">
-        <v>578</v>
-      </c>
-      <c r="CU2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CV2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CW2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CX2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CY2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CZ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DA2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DB2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DC2" t="s">
-        <v>606</v>
-      </c>
-      <c r="DD2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DE2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DF2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DG2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DH2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DI2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DJ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DK2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DL2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DM2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DN2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DO2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DP2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DQ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DR2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DS2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DT2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DU2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DV2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DW2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DX2" t="s">
-        <v>607</v>
-      </c>
-      <c r="DY2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DZ2" t="s">
-        <v>608</v>
-      </c>
-      <c r="EA2" t="s">
-        <v>609</v>
-      </c>
-      <c r="EB2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EC2" t="s">
-        <v>36</v>
-      </c>
-      <c r="ED2" t="s">
-        <v>610</v>
-      </c>
-      <c r="EE2" t="s">
-        <v>611</v>
-      </c>
-      <c r="EF2" t="s">
-        <v>612</v>
-      </c>
-      <c r="EG2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EH2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EI2" t="s">
-        <v>613</v>
-      </c>
-      <c r="EJ2" t="s">
-        <v>614</v>
-      </c>
-      <c r="EK2" t="s">
-        <v>615</v>
-      </c>
-      <c r="EL2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EM2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EN2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EO2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EP2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EQ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="ER2" t="s">
-        <v>583</v>
-      </c>
       <c r="ES2" t="s">
         <v>36</v>
       </c>
@@ -12150,19 +12260,19 @@
         <v>36</v>
       </c>
       <c r="EV2" t="s">
-        <v>616</v>
+        <v>618</v>
       </c>
       <c r="EW2" t="s">
-        <v>617</v>
+        <v>619</v>
       </c>
       <c r="EX2" t="s">
-        <v>618</v>
+        <v>620</v>
       </c>
       <c r="EY2" t="s">
         <v>36</v>
       </c>
       <c r="EZ2" t="s">
-        <v>619</v>
+        <v>621</v>
       </c>
       <c r="FA2" t="s">
         <v>36</v>
@@ -12193,10 +12303,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>620</v>
+        <v>622</v>
       </c>
       <c r="C1" t="s">
-        <v>621</v>
+        <v>623</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>